<commit_message>
Added backend calls for AddOrEditUserWindow
</commit_message>
<xml_diff>
--- a/database/test.xlsx
+++ b/database/test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E749561D-69D1-F44B-A9AD-D0EB9C228B00}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="18200" windowHeight="8020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Person A</t>
   </si>
@@ -57,12 +58,15 @@
   </si>
   <si>
     <t>bin</t>
+  </si>
+  <si>
+    <t>Top-secret</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,6 +193,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -224,6 +245,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,16 +437,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -419,7 +457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -430,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -441,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -459,24 +497,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -484,7 +525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -492,7 +533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Added a method to get permission list by ID number.
* Also disgusting support for remapping permissions.
* Permission remap only works with add_person, if setting or
	* removing permission only the ones called will have an effect.
</commit_message>
<xml_diff>
--- a/database/test.xlsx
+++ b/database/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="people" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Person A</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>bin</t>
+  </si>
+  <si>
+    <t>Top-secret</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -460,31 +463,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -492,7 +501,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
more progress on load already existing user
</commit_message>
<xml_diff>
--- a/database/test.xlsx
+++ b/database/test.xlsx
@@ -1,90 +1,91 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E749561D-69D1-F44B-A9AD-D0EB9C228B00}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18200" windowHeight="8020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="people" sheetId="1" r:id="rId1"/>
-    <sheet name="clearance" sheetId="2" r:id="rId2"/>
+    <sheet name="clearance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="people" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Secret</t>
+  </si>
+  <si>
+    <t>Top-secret</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>numbers</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
   <si>
     <t>Person A</t>
   </si>
   <si>
+    <t>aaa</t>
+  </si>
+  <si>
     <t>Person B</t>
   </si>
   <si>
+    <t>bbb</t>
+  </si>
+  <si>
     <t>Person C</t>
   </si>
   <si>
-    <t>Secret</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
     <t>ccc</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>names</t>
-  </si>
-  <si>
-    <t>numbers</t>
-  </si>
-  <si>
-    <t>bin</t>
-  </si>
-  <si>
-    <t>Top-secret</t>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,28 +93,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -160,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -192,27 +192,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,24 +226,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,110 +401,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>123</v>
+      </c>
+      <c r="B2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="n">
+        <v>222</v>
+      </c>
+      <c r="C3" t="s"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s"/>
+      <c r="C4" t="s"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s"/>
+      <c r="C5" t="s"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>222</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>222</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1"/>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>